<commit_message>
Update to shorter top node-names Some typos Some link updates
</commit_message>
<xml_diff>
--- a/diseaseNetwork/2018-02-26_shorter_names.xlsx
+++ b/diseaseNetwork/2018-02-26_shorter_names.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FOLK\Documents\Work\Bioinformatics\2018-02-12_future-genomics\lasse_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FOLK\Documents\Work\Bioinformatics\2018-05-25_real-impute-me\diseaseNetwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -102,9 +102,6 @@
     <t>Blood-related</t>
   </si>
   <si>
-    <t>Diabetes</t>
-  </si>
-  <si>
     <t>Psychiatric</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>XXII: Codes for special purposes</t>
+  </si>
+  <si>
+    <t>Diabetes etc</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -589,7 +589,7 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -600,7 +600,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -611,7 +611,7 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -619,10 +619,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,10 +630,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -641,10 +641,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,10 +652,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,10 +663,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -674,10 +674,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,10 +685,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,10 +696,10 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,10 +707,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,10 +718,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -729,10 +729,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -740,10 +740,10 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,10 +751,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,10 +762,10 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,10 +773,10 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -784,10 +784,10 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -795,10 +795,10 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -806,10 +806,10 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -817,10 +817,10 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on implementing rare-diseases into disease network module
</commit_message>
<xml_diff>
--- a/diseaseNetwork/2018-02-26_shorter_names.xlsx
+++ b/diseaseNetwork/2018-02-26_shorter_names.xlsx
@@ -225,7 +225,7 @@
     <t>XXII: Codes for special purposes</t>
   </si>
   <si>
-    <t>Diabetes etc</t>
+    <t>Metabolic diseases</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>